<commit_message>
modified structConvert file so it works with more complicated cases; changed names of functions so it is easier to calle
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16780" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="13620" yWindow="440" windowWidth="16780" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,13 @@
     <t>H2O</t>
   </si>
   <si>
-    <t>O2</t>
+    <t>Ca</t>
   </si>
   <si>
-    <t>CH4</t>
+    <t>Ca(OH)2</t>
   </si>
   <si>
-    <t>CO2</t>
+    <t>H2</t>
   </si>
 </sst>
 </file>
@@ -356,23 +356,23 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need a README and a TEST file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -27,18 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Na2CO3</t>
+    <t>H2O</t>
   </si>
   <si>
-    <t>HCl</t>
+    <t>H2</t>
   </si>
   <si>
-    <t>NaCl</t>
-  </si>
-  <si>
-    <t>H2CO3</t>
+    <t>O2</t>
   </si>
 </sst>
 </file>
@@ -353,15 +350,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -371,9 +368,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>